<commit_message>
Update Monster and skills and Collision
</commit_message>
<xml_diff>
--- a/DevFolder/메이플스토리_일정표.xlsx
+++ b/DevFolder/메이플스토리_일정표.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\MapleStory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\MapleStory\DevFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543328FD-6B2C-4433-A6B1-83493C8057F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72681C90-91E2-4493-9DD9-4A820054F4D5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{48DBF8EE-EB68-463B-A5EB-7D5C83FA0543}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{48DBF8EE-EB68-463B-A5EB-7D5C83FA0543}"/>
   </bookViews>
   <sheets>
     <sheet name="개발환경 및 제약사항" sheetId="2" r:id="rId1"/>
     <sheet name="메이플스토리 1주차 일정표" sheetId="1" r:id="rId2"/>
+    <sheet name="메이플스토리 2주차 일정표" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>오늘 한 일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -130,6 +131,72 @@
   </si>
   <si>
     <t>함수, 클래스명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 유한상태기계 순서도 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태가 너무 많아서 생각보다 
+처리해줘야 할 일들이 많았다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터의 상태와 점프 시 상태를 
+같이 처리해주는게 쉽지 않았다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터 움직임 구현 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 씬 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라 클래스 작성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라 클래스를 작성하여 캐릭터의 움직임을 따라가게했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라가 좌, 우, 상, 하의 끝에 도달했을 때 정지시켜줘야하고
+캐릭터의 위치만 이동시켜줘야하는 조건처리에서 고전했다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 씬의 이미지를 찾았다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>새로운 씬의 맵 타일 충돌처리와
+미니맵을 만들었다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사다리와의 충돌처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사다리와의 충돌처리 구현 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사다리에 매달려서 사다리 끝에 닿았을 때
+정상적으로 이동하지 않는 문제 발생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매달리기 애니메이션이 제대로 출력되지 않는 
+문제 발생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로딩씬 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -233,7 +300,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -264,28 +331,31 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,10 +685,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="17"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -657,10 +727,10 @@
       <c r="C8" s="9"/>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="17"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -672,35 +742,35 @@
     </row>
     <row r="12" spans="2:3" ht="33" x14ac:dyDescent="0.3">
       <c r="B12" s="1"/>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="15" t="s">
         <v>22</v>
       </c>
     </row>
@@ -718,15 +788,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4A9FA6-C581-43DE-B53E-F8FC0A1B065C}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -745,24 +819,12 @@
       <c r="F1" s="4">
         <v>44330</v>
       </c>
-      <c r="G1" s="4">
-        <v>44331</v>
-      </c>
-      <c r="H1" s="4">
-        <v>44332</v>
-      </c>
-      <c r="I1" s="4">
-        <v>44333</v>
-      </c>
-      <c r="J1" s="4">
-        <v>44334</v>
-      </c>
-      <c r="K1" s="4">
-        <v>44335</v>
-      </c>
-      <c r="L1" s="4">
-        <v>44336</v>
-      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -770,6 +832,9 @@
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -794,6 +859,18 @@
       <c r="A6" s="6" t="s">
         <v>0</v>
       </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
@@ -804,13 +881,24 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
@@ -819,6 +907,129 @@
       <c r="A13" s="3"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0673F144-9B16-45E1-8A04-8D6FA74D96F1}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B1" s="4">
+        <v>44331</v>
+      </c>
+      <c r="C1" s="4">
+        <v>44332</v>
+      </c>
+      <c r="D1" s="4">
+        <v>44333</v>
+      </c>
+      <c r="E1" s="4">
+        <v>44334</v>
+      </c>
+      <c r="F1" s="4">
+        <v>44335</v>
+      </c>
+      <c r="G1" s="4">
+        <v>44336</v>
+      </c>
+      <c r="H1" s="4">
+        <v>44337</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="C11" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
     </row>
   </sheetData>

</xml_diff>